<commit_message>
new and modified test data excel files
</commit_message>
<xml_diff>
--- a/test-data/Metadata_template-example-for-SOCAT-FULL_TEST.xlsx
+++ b/test-data/Metadata_template-example-for-SOCAT-FULL_TEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamb/oxy-work/OMD/OAPMetadataEditor/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D889B3-C7D2-8542-9A6E-15C6A0FAB974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCD8E48-AF59-EC44-9AEC-E864307C6E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26180" yWindow="460" windowWidth="24060" windowHeight="26560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3729,15 +3729,6 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3839,6 +3830,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4132,8 +4132,8 @@
   </sheetPr>
   <dimension ref="A1:X267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A254" sqref="A254:C267"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4148,12 +4148,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="244" t="s">
         <v>532</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="210"/>
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="246"/>
       <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4178,7 +4178,7 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="211" t="s">
+      <c r="C3" s="208" t="s">
         <v>583</v>
       </c>
       <c r="D3" s="109">
@@ -4318,7 +4318,7 @@
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="212" t="s">
+      <c r="C8" s="209" t="s">
         <v>588</v>
       </c>
       <c r="D8" s="103">
@@ -4346,7 +4346,7 @@
       <c r="B9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="211" t="s">
+      <c r="C9" s="208" t="s">
         <v>589</v>
       </c>
       <c r="D9" s="70">
@@ -4374,7 +4374,7 @@
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="213" t="s">
+      <c r="C10" s="210" t="s">
         <v>590</v>
       </c>
       <c r="D10" s="71" t="s">
@@ -4402,7 +4402,7 @@
       <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="211" t="s">
+      <c r="C11" s="208" t="s">
         <v>591</v>
       </c>
       <c r="D11" s="70">
@@ -4458,7 +4458,7 @@
       <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="214" t="s">
+      <c r="C13" s="211" t="s">
         <v>593</v>
       </c>
       <c r="D13" s="70">
@@ -4486,7 +4486,7 @@
       <c r="B14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="215" t="s">
+      <c r="C14" s="212" t="s">
         <v>594</v>
       </c>
       <c r="D14" s="70">
@@ -4514,7 +4514,7 @@
       <c r="B15" s="139" t="s">
         <v>537</v>
       </c>
-      <c r="C15" s="216" t="s">
+      <c r="C15" s="213" t="s">
         <v>192</v>
       </c>
       <c r="D15" s="145">
@@ -4542,7 +4542,7 @@
       <c r="B16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="212" t="s">
+      <c r="C16" s="209" t="s">
         <v>595</v>
       </c>
       <c r="D16" s="107">
@@ -4570,7 +4570,7 @@
       <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="211" t="s">
+      <c r="C17" s="208" t="s">
         <v>596</v>
       </c>
       <c r="D17" s="71">
@@ -4598,7 +4598,7 @@
       <c r="B18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="213" t="s">
+      <c r="C18" s="210" t="s">
         <v>597</v>
       </c>
       <c r="D18" s="71" t="s">
@@ -4626,7 +4626,7 @@
       <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="211" t="s">
+      <c r="C19" s="208" t="s">
         <v>598</v>
       </c>
       <c r="D19" s="71">
@@ -4682,7 +4682,7 @@
       <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="214" t="s">
+      <c r="C21" s="211" t="s">
         <v>600</v>
       </c>
       <c r="D21" s="71">
@@ -4710,7 +4710,7 @@
       <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="215" t="s">
+      <c r="C22" s="212" t="s">
         <v>601</v>
       </c>
       <c r="D22" s="71">
@@ -4738,7 +4738,7 @@
       <c r="B23" s="149" t="s">
         <v>534</v>
       </c>
-      <c r="C23" s="216" t="s">
+      <c r="C23" s="213" t="s">
         <v>193</v>
       </c>
       <c r="D23" s="150">
@@ -4766,7 +4766,7 @@
       <c r="B24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="217"/>
+      <c r="C24" s="214"/>
       <c r="D24" s="107">
         <v>6.1</v>
       </c>
@@ -4792,7 +4792,7 @@
       <c r="B25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="211"/>
+      <c r="C25" s="208"/>
       <c r="D25" s="71">
         <v>6.2</v>
       </c>
@@ -4818,7 +4818,7 @@
       <c r="B26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="213"/>
+      <c r="C26" s="210"/>
       <c r="D26" s="71" t="s">
         <v>12</v>
       </c>
@@ -4844,7 +4844,7 @@
       <c r="B27" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="211"/>
+      <c r="C27" s="208"/>
       <c r="D27" s="71">
         <v>6.4</v>
       </c>
@@ -4896,7 +4896,7 @@
       <c r="B29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="218"/>
+      <c r="C29" s="215"/>
       <c r="D29" s="71">
         <v>6.6</v>
       </c>
@@ -4922,7 +4922,7 @@
       <c r="B30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="219"/>
+      <c r="C30" s="216"/>
       <c r="D30" s="71">
         <v>6.7</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="B31" s="149" t="s">
         <v>535</v>
       </c>
-      <c r="C31" s="216"/>
+      <c r="C31" s="213"/>
       <c r="D31" s="150">
         <v>6.8</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="B32" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="212" t="s">
+      <c r="C32" s="209" t="s">
         <v>602</v>
       </c>
       <c r="D32" s="103">
@@ -5002,7 +5002,7 @@
       <c r="B33" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="211" t="s">
+      <c r="C33" s="208" t="s">
         <v>603</v>
       </c>
       <c r="D33" s="70">
@@ -5030,7 +5030,7 @@
       <c r="B34" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="213" t="s">
+      <c r="C34" s="210" t="s">
         <v>604</v>
       </c>
       <c r="D34" s="71">
@@ -5058,7 +5058,7 @@
       <c r="B35" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="211" t="s">
+      <c r="C35" s="208" t="s">
         <v>605</v>
       </c>
       <c r="D35" s="70">
@@ -5114,7 +5114,7 @@
       <c r="B37" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="214" t="s">
+      <c r="C37" s="211" t="s">
         <v>607</v>
       </c>
       <c r="D37" s="70">
@@ -5142,7 +5142,7 @@
       <c r="B38" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="215" t="s">
+      <c r="C38" s="212" t="s">
         <v>608</v>
       </c>
       <c r="D38" s="70">
@@ -5170,7 +5170,7 @@
       <c r="B39" s="153" t="s">
         <v>536</v>
       </c>
-      <c r="C39" s="216" t="s">
+      <c r="C39" s="213" t="s">
         <v>530</v>
       </c>
       <c r="D39" s="140">
@@ -5226,7 +5226,7 @@
       <c r="B41" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="220" t="s">
+      <c r="C41" s="217" t="s">
         <v>610</v>
       </c>
       <c r="D41" s="77">
@@ -5254,7 +5254,7 @@
       <c r="B42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="221" t="s">
+      <c r="C42" s="218" t="s">
         <v>611</v>
       </c>
       <c r="D42" s="78">
@@ -5310,7 +5310,7 @@
       <c r="B44" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="222" t="s">
+      <c r="C44" s="219" t="s">
         <v>613</v>
       </c>
       <c r="D44" s="74">
@@ -5558,7 +5558,7 @@
       <c r="B53" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="222" t="s">
+      <c r="C53" s="219" t="s">
         <v>617</v>
       </c>
       <c r="D53" s="72">
@@ -5586,7 +5586,7 @@
       <c r="B54" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="223" t="s">
+      <c r="C54" s="220" t="s">
         <v>618</v>
       </c>
       <c r="D54" s="107">
@@ -5614,7 +5614,7 @@
       <c r="B55" s="149" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="224" t="s">
+      <c r="C55" s="221" t="s">
         <v>533</v>
       </c>
       <c r="D55" s="181">
@@ -5670,7 +5670,7 @@
       <c r="B57" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="224" t="s">
+      <c r="C57" s="221" t="s">
         <v>204</v>
       </c>
       <c r="D57" s="181">
@@ -5726,7 +5726,7 @@
       <c r="B59" s="154" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="225" t="s">
+      <c r="C59" s="222" t="s">
         <v>306</v>
       </c>
       <c r="D59" s="150">
@@ -5810,7 +5810,7 @@
       <c r="B62" s="149" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="224" t="s">
+      <c r="C62" s="221" t="s">
         <v>203</v>
       </c>
       <c r="D62" s="156">
@@ -5838,7 +5838,7 @@
       <c r="B63" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="212" t="s">
+      <c r="C63" s="209" t="s">
         <v>623</v>
       </c>
       <c r="D63" s="76">
@@ -5894,7 +5894,7 @@
       <c r="B65" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="222" t="s">
+      <c r="C65" s="219" t="s">
         <v>625</v>
       </c>
       <c r="D65" s="78">
@@ -5922,7 +5922,7 @@
       <c r="B66" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="211" t="s">
+      <c r="C66" s="208" t="s">
         <v>626</v>
       </c>
       <c r="D66" s="105">
@@ -5950,7 +5950,7 @@
       <c r="B67" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="226" t="s">
+      <c r="C67" s="223" t="s">
         <v>209</v>
       </c>
       <c r="D67" s="158">
@@ -8913,7 +8913,7 @@
         <v>550</v>
       </c>
       <c r="C180" s="166" t="s">
-        <v>238</v>
+        <v>509</v>
       </c>
       <c r="D180" s="190">
         <v>24.9</v>
@@ -9080,7 +9080,7 @@
       <c r="B186" s="149" t="s">
         <v>555</v>
       </c>
-      <c r="C186" s="224" t="s">
+      <c r="C186" s="221" t="s">
         <v>294</v>
       </c>
       <c r="D186" s="191">
@@ -9500,7 +9500,7 @@
       <c r="B201" s="28" t="s">
         <v>570</v>
       </c>
-      <c r="C201" s="227" t="s">
+      <c r="C201" s="224" t="s">
         <v>658</v>
       </c>
       <c r="D201" s="31">
@@ -9528,7 +9528,7 @@
       <c r="B202" s="149" t="s">
         <v>571</v>
       </c>
-      <c r="C202" s="228" t="s">
+      <c r="C202" s="225" t="s">
         <v>228</v>
       </c>
       <c r="D202" s="191">
@@ -9808,7 +9808,7 @@
       <c r="B212" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="C212" s="227" t="s">
+      <c r="C212" s="224" t="s">
         <v>666</v>
       </c>
       <c r="D212" s="111">
@@ -9836,7 +9836,7 @@
       <c r="B213" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="C213" s="229" t="s">
+      <c r="C213" s="226" t="s">
         <v>667</v>
       </c>
       <c r="D213" s="98">
@@ -9864,7 +9864,7 @@
       <c r="B214" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C214" s="211" t="s">
+      <c r="C214" s="208" t="s">
         <v>668</v>
       </c>
       <c r="D214" s="103">
@@ -9892,7 +9892,7 @@
       <c r="B215" s="139" t="s">
         <v>159</v>
       </c>
-      <c r="C215" s="230" t="s">
+      <c r="C215" s="227" t="s">
         <v>211</v>
       </c>
       <c r="D215" s="162">
@@ -9920,7 +9920,7 @@
       <c r="B216" s="139" t="s">
         <v>160</v>
       </c>
-      <c r="C216" s="211" t="s">
+      <c r="C216" s="208" t="s">
         <v>669</v>
       </c>
       <c r="D216" s="163">
@@ -9947,7 +9947,7 @@
       <c r="B217" s="139" t="s">
         <v>161</v>
       </c>
-      <c r="C217" s="230" t="s">
+      <c r="C217" s="227" t="s">
         <v>241</v>
       </c>
       <c r="D217" s="193">
@@ -9974,7 +9974,7 @@
       <c r="B218" s="139" t="s">
         <v>162</v>
       </c>
-      <c r="C218" s="211" t="s">
+      <c r="C218" s="208" t="s">
         <v>670</v>
       </c>
       <c r="D218" s="162">
@@ -10030,7 +10030,7 @@
       <c r="B220" s="149" t="s">
         <v>166</v>
       </c>
-      <c r="C220" s="231" t="s">
+      <c r="C220" s="228" t="s">
         <v>509</v>
       </c>
       <c r="D220" s="181">
@@ -10058,7 +10058,7 @@
       <c r="B221" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="C221" s="232" t="s">
+      <c r="C221" s="229" t="s">
         <v>672</v>
       </c>
       <c r="D221" s="79">
@@ -10086,7 +10086,7 @@
       <c r="B222" s="149" t="s">
         <v>516</v>
       </c>
-      <c r="C222" s="233" t="s">
+      <c r="C222" s="230" t="s">
         <v>462</v>
       </c>
       <c r="D222" s="181">
@@ -10114,7 +10114,7 @@
       <c r="B223" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C223" s="234" t="s">
+      <c r="C223" s="231" t="s">
         <v>673</v>
       </c>
       <c r="D223" s="30">
@@ -10142,7 +10142,7 @@
       <c r="B224" s="149" t="s">
         <v>164</v>
       </c>
-      <c r="C224" s="228">
+      <c r="C224" s="225">
         <v>1</v>
       </c>
       <c r="D224" s="185">
@@ -10170,7 +10170,7 @@
       <c r="B225" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C225" s="227" t="s">
+      <c r="C225" s="224" t="s">
         <v>674</v>
       </c>
       <c r="D225" s="111">
@@ -10198,7 +10198,7 @@
       <c r="B226" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="C226" s="229" t="s">
+      <c r="C226" s="226" t="s">
         <v>675</v>
       </c>
       <c r="D226" s="116">
@@ -10226,7 +10226,7 @@
       <c r="B227" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C227" s="211" t="s">
+      <c r="C227" s="208" t="s">
         <v>676</v>
       </c>
       <c r="D227" s="103">
@@ -10254,7 +10254,7 @@
       <c r="B228" s="139" t="s">
         <v>170</v>
       </c>
-      <c r="C228" s="230" t="s">
+      <c r="C228" s="227" t="s">
         <v>211</v>
       </c>
       <c r="D228" s="163">
@@ -10282,7 +10282,7 @@
       <c r="B229" s="139" t="s">
         <v>171</v>
       </c>
-      <c r="C229" s="211" t="s">
+      <c r="C229" s="208" t="s">
         <v>677</v>
       </c>
       <c r="D229" s="163">
@@ -10310,7 +10310,7 @@
       <c r="B230" s="139" t="s">
         <v>172</v>
       </c>
-      <c r="C230" s="230" t="s">
+      <c r="C230" s="227" t="s">
         <v>241</v>
       </c>
       <c r="D230" s="163">
@@ -10338,7 +10338,7 @@
       <c r="B231" s="139" t="s">
         <v>173</v>
       </c>
-      <c r="C231" s="211" t="s">
+      <c r="C231" s="208" t="s">
         <v>678</v>
       </c>
       <c r="D231" s="163">
@@ -10394,7 +10394,7 @@
       <c r="B233" s="149" t="s">
         <v>177</v>
       </c>
-      <c r="C233" s="231" t="s">
+      <c r="C233" s="228" t="s">
         <v>509</v>
       </c>
       <c r="D233" s="181">
@@ -10422,7 +10422,7 @@
       <c r="B234" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="C234" s="232" t="s">
+      <c r="C234" s="229" t="s">
         <v>680</v>
       </c>
       <c r="D234" s="71">
@@ -10450,7 +10450,7 @@
       <c r="B235" s="149" t="s">
         <v>518</v>
       </c>
-      <c r="C235" s="233" t="s">
+      <c r="C235" s="230" t="s">
         <v>462</v>
       </c>
       <c r="D235" s="181">
@@ -10478,7 +10478,7 @@
       <c r="B236" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C236" s="234" t="s">
+      <c r="C236" s="231" t="s">
         <v>681</v>
       </c>
       <c r="D236" s="27">
@@ -10506,7 +10506,7 @@
       <c r="B237" s="149" t="s">
         <v>175</v>
       </c>
-      <c r="C237" s="228">
+      <c r="C237" s="225">
         <v>1</v>
       </c>
       <c r="D237" s="185">
@@ -10534,7 +10534,7 @@
       <c r="B238" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C238" s="227" t="s">
+      <c r="C238" s="224" t="s">
         <v>682</v>
       </c>
       <c r="D238" s="111">
@@ -10562,7 +10562,7 @@
       <c r="B239" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C239" s="229" t="s">
+      <c r="C239" s="226" t="s">
         <v>683</v>
       </c>
       <c r="D239" s="98">
@@ -10590,7 +10590,7 @@
       <c r="B240" s="118" t="s">
         <v>180</v>
       </c>
-      <c r="C240" s="212" t="s">
+      <c r="C240" s="209" t="s">
         <v>684</v>
       </c>
       <c r="D240" s="103">
@@ -10618,7 +10618,7 @@
       <c r="B241" s="119" t="s">
         <v>181</v>
       </c>
-      <c r="C241" s="211" t="s">
+      <c r="C241" s="208" t="s">
         <v>685</v>
       </c>
       <c r="D241" s="70">
@@ -10646,7 +10646,7 @@
       <c r="B242" s="160" t="s">
         <v>182</v>
       </c>
-      <c r="C242" s="230" t="s">
+      <c r="C242" s="227" t="s">
         <v>211</v>
       </c>
       <c r="D242" s="162">
@@ -10674,7 +10674,7 @@
       <c r="B243" s="119" t="s">
         <v>183</v>
       </c>
-      <c r="C243" s="211" t="s">
+      <c r="C243" s="208" t="s">
         <v>686</v>
       </c>
       <c r="D243" s="70">
@@ -10702,7 +10702,7 @@
       <c r="B244" s="160" t="s">
         <v>184</v>
       </c>
-      <c r="C244" s="230" t="s">
+      <c r="C244" s="227" t="s">
         <v>241</v>
       </c>
       <c r="D244" s="163">
@@ -10730,7 +10730,7 @@
       <c r="B245" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C245" s="211" t="s">
+      <c r="C245" s="208" t="s">
         <v>687</v>
       </c>
       <c r="D245" s="162">
@@ -10786,7 +10786,7 @@
       <c r="B247" s="168" t="s">
         <v>189</v>
       </c>
-      <c r="C247" s="231" t="s">
+      <c r="C247" s="228" t="s">
         <v>509</v>
       </c>
       <c r="D247" s="181">
@@ -10814,7 +10814,7 @@
       <c r="B248" s="120" t="s">
         <v>519</v>
       </c>
-      <c r="C248" s="232" t="s">
+      <c r="C248" s="229" t="s">
         <v>689</v>
       </c>
       <c r="D248" s="71">
@@ -10842,7 +10842,7 @@
       <c r="B249" s="168" t="s">
         <v>520</v>
       </c>
-      <c r="C249" s="233" t="s">
+      <c r="C249" s="230" t="s">
         <v>462</v>
       </c>
       <c r="D249" s="182">
@@ -10870,7 +10870,7 @@
       <c r="B250" s="120" t="s">
         <v>188</v>
       </c>
-      <c r="C250" s="234" t="s">
+      <c r="C250" s="231" t="s">
         <v>690</v>
       </c>
       <c r="D250" s="27">
@@ -10898,7 +10898,7 @@
       <c r="B251" s="168" t="s">
         <v>187</v>
       </c>
-      <c r="C251" s="228">
+      <c r="C251" s="225">
         <v>1</v>
       </c>
       <c r="D251" s="182">
@@ -10926,7 +10926,7 @@
       <c r="B252" s="120" t="s">
         <v>190</v>
       </c>
-      <c r="C252" s="227" t="s">
+      <c r="C252" s="224" t="s">
         <v>691</v>
       </c>
       <c r="D252" s="27">
@@ -10954,7 +10954,7 @@
       <c r="B253" s="121" t="s">
         <v>191</v>
       </c>
-      <c r="C253" s="229" t="s">
+      <c r="C253" s="226" t="s">
         <v>692</v>
       </c>
       <c r="D253" s="98">
@@ -10976,76 +10976,76 @@
       <c r="R253" s="16"/>
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A254" s="235">
+      <c r="A254" s="232">
         <v>227</v>
       </c>
-      <c r="B254" s="236" t="s">
+      <c r="B254" s="233" t="s">
         <v>693</v>
       </c>
-      <c r="C254" s="212" t="s">
+      <c r="C254" s="209" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="255" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A255" s="237">
+      <c r="A255" s="234">
         <v>228</v>
       </c>
-      <c r="B255" s="238" t="s">
+      <c r="B255" s="235" t="s">
         <v>695</v>
       </c>
-      <c r="C255" s="211" t="s">
+      <c r="C255" s="208" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="256" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A256" s="239">
+      <c r="A256" s="236">
         <v>229</v>
       </c>
-      <c r="B256" s="240" t="s">
+      <c r="B256" s="237" t="s">
         <v>697</v>
       </c>
-      <c r="C256" s="230" t="s">
+      <c r="C256" s="227" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257" s="237">
+      <c r="A257" s="234">
         <v>230</v>
       </c>
-      <c r="B257" s="238" t="s">
+      <c r="B257" s="235" t="s">
         <v>698</v>
       </c>
-      <c r="C257" s="211" t="s">
+      <c r="C257" s="208" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258" s="239">
+      <c r="A258" s="236">
         <v>231</v>
       </c>
-      <c r="B258" s="240" t="s">
+      <c r="B258" s="237" t="s">
         <v>700</v>
       </c>
-      <c r="C258" s="230" t="s">
+      <c r="C258" s="227" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A259" s="237">
+      <c r="A259" s="234">
         <v>232</v>
       </c>
-      <c r="B259" s="238" t="s">
+      <c r="B259" s="235" t="s">
         <v>701</v>
       </c>
-      <c r="C259" s="211" t="s">
+      <c r="C259" s="208" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A260" s="241">
+      <c r="A260" s="238">
         <v>233</v>
       </c>
-      <c r="B260" s="242" t="s">
+      <c r="B260" s="239" t="s">
         <v>703</v>
       </c>
       <c r="C260" s="196" t="s">
@@ -11053,79 +11053,79 @@
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A261" s="243">
+      <c r="A261" s="240">
         <v>234</v>
       </c>
-      <c r="B261" s="244" t="s">
+      <c r="B261" s="241" t="s">
         <v>705</v>
       </c>
-      <c r="C261" s="231" t="s">
+      <c r="C261" s="228" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A262" s="241">
+      <c r="A262" s="238">
         <v>235</v>
       </c>
-      <c r="B262" s="242" t="s">
+      <c r="B262" s="239" t="s">
         <v>706</v>
       </c>
-      <c r="C262" s="232" t="s">
+      <c r="C262" s="229" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A263" s="243">
+      <c r="A263" s="240">
         <v>236</v>
       </c>
-      <c r="B263" s="244" t="s">
+      <c r="B263" s="241" t="s">
         <v>708</v>
       </c>
-      <c r="C263" s="233" t="s">
+      <c r="C263" s="230" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A264" s="241">
+      <c r="A264" s="238">
         <v>237</v>
       </c>
-      <c r="B264" s="242" t="s">
+      <c r="B264" s="239" t="s">
         <v>709</v>
       </c>
-      <c r="C264" s="234" t="s">
+      <c r="C264" s="231" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A265" s="243">
+      <c r="A265" s="240">
         <v>238</v>
       </c>
-      <c r="B265" s="244" t="s">
+      <c r="B265" s="241" t="s">
         <v>711</v>
       </c>
-      <c r="C265" s="228">
+      <c r="C265" s="225">
         <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266" s="241">
+      <c r="A266" s="238">
         <v>239</v>
       </c>
-      <c r="B266" s="242" t="s">
+      <c r="B266" s="239" t="s">
         <v>712</v>
       </c>
-      <c r="C266" s="227" t="s">
+      <c r="C266" s="224" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A267" s="245">
+      <c r="A267" s="242">
         <v>240</v>
       </c>
-      <c r="B267" s="246" t="s">
+      <c r="B267" s="243" t="s">
         <v>714</v>
       </c>
-      <c r="C267" s="229" t="s">
+      <c r="C267" s="226" t="s">
         <v>715</v>
       </c>
     </row>

</xml_diff>